<commit_message>
data from jill, augmented by ian
</commit_message>
<xml_diff>
--- a/data/DragonSurvey.xlsx
+++ b/data/DragonSurvey.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="Very Raw Data" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="118">
   <si>
     <t>Dragon Age</t>
   </si>
@@ -285,36 +285,6 @@
   </si>
   <si>
     <t>Last rescue date</t>
-  </si>
-  <si>
-    <t>23/6/1634</t>
-  </si>
-  <si>
-    <t>6/5/1890</t>
-  </si>
-  <si>
-    <t>5/2/1888</t>
-  </si>
-  <si>
-    <t>1/8/1876</t>
-  </si>
-  <si>
-    <t>18/5/1850</t>
-  </si>
-  <si>
-    <t>4/3/1763</t>
-  </si>
-  <si>
-    <t>2/4/1856</t>
-  </si>
-  <si>
-    <t>3/9/1899</t>
-  </si>
-  <si>
-    <t>1/5/1876</t>
-  </si>
-  <si>
-    <t>4/12/1870</t>
   </si>
   <si>
     <t>Colour and Markings</t>
@@ -421,7 +391,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -468,13 +438,13 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -795,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -810,7 +780,7 @@
     <col min="7" max="7" width="21.6640625" style="5" customWidth="1"/>
     <col min="8" max="8" width="51.5" style="5" customWidth="1"/>
     <col min="9" max="9" width="18.5" style="5" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="38" style="2" customWidth="1"/>
     <col min="11" max="11" width="18.5" style="5" customWidth="1"/>
     <col min="12" max="16384" width="8.83203125" style="5"/>
   </cols>
@@ -820,7 +790,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>41</v>
@@ -847,7 +817,7 @@
         <v>84</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -855,10 +825,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>4</v>
@@ -882,7 +852,7 @@
         <v>37104</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -914,7 +884,7 @@
         <v>28752</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -946,7 +916,7 @@
         <v>36089</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -954,7 +924,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
@@ -963,7 +933,7 @@
         <v>182</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="G5" s="5">
         <v>20</v>
@@ -978,7 +948,7 @@
         <v>36621</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -989,7 +959,7 @@
         <v>43</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E6" s="5">
         <v>39</v>
@@ -998,7 +968,7 @@
         <v>79</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>49</v>
@@ -1006,11 +976,11 @@
       <c r="I6" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>85</v>
+      <c r="J6" s="2">
+        <v>12593</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1042,7 +1012,7 @@
         <v>37562</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1050,7 +1020,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>42</v>
@@ -1073,11 +1043,11 @@
       <c r="I9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>86</v>
+      <c r="J9" s="2">
+        <v>32999</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1105,11 +1075,11 @@
       <c r="I10" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>87</v>
+      <c r="J10" s="2">
+        <v>32178</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1120,7 +1090,7 @@
         <v>43</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E11" s="5">
         <v>240</v>
@@ -1141,7 +1111,7 @@
         <v>40403</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1173,7 +1143,7 @@
         <v>36526</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1201,11 +1171,11 @@
       <c r="I13" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>88</v>
+      <c r="J13" s="2">
+        <v>17015</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1237,7 +1207,7 @@
         <v>34807</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1245,7 +1215,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>42</v>
@@ -1272,7 +1242,7 @@
         <v>41531</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1304,7 +1274,7 @@
         <v>36618</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1336,7 +1306,7 @@
         <v>19754</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1356,7 +1326,7 @@
         <v>59</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>58</v>
@@ -1368,7 +1338,7 @@
         <v>23809</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1379,13 +1349,13 @@
         <v>42</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E20" s="5">
         <v>92</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="G20" s="5">
         <v>18</v>
@@ -1400,7 +1370,7 @@
         <v>36926</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1408,7 +1378,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>42</v>
@@ -1431,11 +1401,11 @@
       <c r="I22" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>89</v>
+      <c r="J22" s="2">
+        <v>18401</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1467,7 +1437,7 @@
         <v>22564</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1475,7 +1445,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>5</v>
@@ -1495,11 +1465,11 @@
       <c r="I24" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>90</v>
+      <c r="J24" s="2">
+        <v>23074</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1510,7 +1480,7 @@
         <v>42</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E25" s="5">
         <v>205</v>
@@ -1531,7 +1501,7 @@
         <v>25813</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1559,11 +1529,11 @@
       <c r="I26" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="2">
+        <v>20547</v>
+      </c>
+      <c r="K26" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1595,7 +1565,7 @@
         <v>40461</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1603,7 +1573,7 @@
         <v>30</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>43</v>
@@ -1615,7 +1585,7 @@
         <v>36</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="G29" s="5">
         <v>2</v>
@@ -1630,7 +1600,7 @@
         <v>29291</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1638,7 +1608,7 @@
         <v>31</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>4</v>
@@ -1662,7 +1632,7 @@
         <v>20578</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1694,7 +1664,7 @@
         <v>1473</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -1726,7 +1696,7 @@
         <v>18347</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1734,7 +1704,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>44</v>
@@ -1761,7 +1731,7 @@
         <v>36545</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -1772,7 +1742,7 @@
         <v>43</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E35" s="5">
         <v>154</v>
@@ -1789,11 +1759,11 @@
       <c r="I35" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>92</v>
+      <c r="J35" s="2">
+        <v>36406</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1821,11 +1791,11 @@
       <c r="I36" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>93</v>
+      <c r="J36" s="2">
+        <v>27881</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1857,7 +1827,7 @@
         <v>36855</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1868,7 +1838,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>42</v>
@@ -1895,7 +1865,7 @@
         <v>36163</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1912,7 +1882,7 @@
         <v>154</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="G40" s="7">
         <v>18</v>
@@ -1923,11 +1893,11 @@
       <c r="I40" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="J40" s="3" t="s">
-        <v>94</v>
+      <c r="J40" s="3">
+        <v>25906</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1944,7 +1914,7 @@
         <v>212</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="G41" s="7">
         <v>18</v>
@@ -1959,7 +1929,7 @@
         <v>36939</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1976,7 +1946,7 @@
         <v>150</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G42" s="7">
         <v>11</v>
@@ -1991,7 +1961,7 @@
         <v>40233</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>